<commit_message>
feat: :sparkles: actualizacion y cambios
se actualizaron las normalizaciones , modelo fisico y creacion de base de datos y se agrego las funciones
</commit_message>
<xml_diff>
--- a/NORMALIZACION_COMPLETA.xlsx
+++ b/NORMALIZACION_COMPLETA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\PROGRAMACION\MYSQL2\EDWIND\Sistema de Gestión Inmobiliaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089755B5-2BB6-43BB-8525-0498772560E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B297DAD-1549-41C5-8F92-28D23B660226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabla sin normalizar" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="370">
   <si>
     <t>SISTEMA INMOBILIARIO – TABLA SIN NORMALIZAR (0FN)</t>
   </si>
@@ -906,9 +906,6 @@
     <t>PROP-04</t>
   </si>
   <si>
-    <t>CIU-06</t>
-  </si>
-  <si>
     <t>BAR-06</t>
   </si>
   <si>
@@ -993,9 +990,6 @@
     <t>Fecha_Evento</t>
   </si>
   <si>
-    <t>Usuario</t>
-  </si>
-  <si>
     <t>Fecha_Hora</t>
   </si>
   <si>
@@ -1141,13 +1135,16 @@
   </si>
   <si>
     <t>2024-06-12 16:01:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Usuario_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1250,6 +1247,16 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1322,7 +1329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1383,6 +1390,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1657,7 +1670,7 @@
       <selection activeCell="J7" sqref="J7:AJ13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="11" max="11" width="15.08984375" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
@@ -1680,7 +1693,7 @@
     <col min="36" max="36" width="22.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:48" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:48" ht="16.5">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1732,7 +1745,7 @@
       <c r="AU4" s="12"/>
       <c r="AV4" s="12"/>
     </row>
-    <row r="7" spans="1:48" ht="25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:48" ht="25">
       <c r="J7" s="7" t="s">
         <v>1</v>
       </c>
@@ -1815,7 +1828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:48" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:48" ht="54.5" customHeight="1">
       <c r="J8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1898,7 +1911,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:48" ht="65" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:48" ht="65">
       <c r="J9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1981,7 +1994,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:48" ht="65" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:48" ht="65">
       <c r="J10" s="1" t="s">
         <v>70</v>
       </c>
@@ -2064,7 +2077,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:48" ht="65" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:48" ht="65">
       <c r="J11" s="1" t="s">
         <v>85</v>
       </c>
@@ -2147,7 +2160,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:48" ht="52" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:48" ht="52">
       <c r="J12" s="1" t="s">
         <v>99</v>
       </c>
@@ -2230,7 +2243,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:48" ht="65" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:48" ht="65">
       <c r="J13" s="1" t="s">
         <v>112</v>
       </c>
@@ -2325,11 +2338,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV120"/>
   <sheetViews>
-    <sheetView topLeftCell="J18" zoomScale="62" zoomScaleNormal="71" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="62" zoomScaleNormal="71" workbookViewId="0">
       <selection activeCell="J38" sqref="J38:K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.453125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="18.54296875" customWidth="1"/>
     <col min="2" max="2" width="13.6328125" customWidth="1"/>
@@ -2348,7 +2361,7 @@
     <col min="15" max="15" width="22.453125" customWidth="1"/>
     <col min="16" max="16" width="18.81640625" customWidth="1"/>
     <col min="17" max="17" width="17.81640625" customWidth="1"/>
-    <col min="18" max="18" width="14" customWidth="1"/>
+    <col min="18" max="18" width="22.08984375" customWidth="1"/>
     <col min="19" max="19" width="17.36328125" customWidth="1"/>
     <col min="20" max="20" width="14.6328125" customWidth="1"/>
     <col min="21" max="21" width="14.08984375" customWidth="1"/>
@@ -2372,16 +2385,16 @@
     <col min="41" max="41" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:48" ht="24.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:48" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:48" ht="52.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:48" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:48" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:48" ht="35.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:48" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:48" ht="16.5" customHeight="1"/>
+    <row r="2" spans="1:48" ht="24.75" customHeight="1"/>
+    <row r="3" spans="1:48" ht="33.75" customHeight="1"/>
+    <row r="4" spans="1:48" ht="52.5" customHeight="1"/>
+    <row r="5" spans="1:48" ht="33" customHeight="1"/>
+    <row r="6" spans="1:48" ht="36" customHeight="1"/>
+    <row r="7" spans="1:48" ht="35.25" customHeight="1"/>
+    <row r="8" spans="1:48" ht="30" customHeight="1"/>
+    <row r="9" spans="1:48" ht="25.5" customHeight="1"/>
+    <row r="13" spans="1:48">
       <c r="A13" s="16" t="s">
         <v>124</v>
       </c>
@@ -2433,7 +2446,7 @@
       <c r="AU13" s="16"/>
       <c r="AV13" s="16"/>
     </row>
-    <row r="17" spans="1:33" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:33" ht="24.75" customHeight="1">
       <c r="D17" s="7" t="s">
         <v>125</v>
       </c>
@@ -2525,7 +2538,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:33" ht="27" customHeight="1">
       <c r="D18" s="2" t="s">
         <v>28</v>
       </c>
@@ -2617,7 +2630,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:33" ht="26.25" customHeight="1">
       <c r="D19" s="2" t="s">
         <v>28</v>
       </c>
@@ -2709,7 +2722,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:33" ht="25.5" customHeight="1">
       <c r="D20" s="2" t="s">
         <v>28</v>
       </c>
@@ -2801,7 +2814,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:33" ht="24" customHeight="1">
       <c r="D21" s="2" t="s">
         <v>51</v>
       </c>
@@ -2893,7 +2906,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:33" ht="24.75" customHeight="1">
       <c r="D22" s="2" t="s">
         <v>70</v>
       </c>
@@ -2985,7 +2998,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:33" ht="27" customHeight="1">
       <c r="D23" s="2" t="s">
         <v>70</v>
       </c>
@@ -3077,7 +3090,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:33" ht="24" customHeight="1">
       <c r="D24" s="2" t="s">
         <v>85</v>
       </c>
@@ -3169,7 +3182,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:33" ht="29.25" customHeight="1">
       <c r="D25" s="2" t="s">
         <v>99</v>
       </c>
@@ -3261,7 +3274,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:33" ht="25.5" customHeight="1">
       <c r="D26" s="2" t="s">
         <v>112</v>
       </c>
@@ -3353,7 +3366,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:33">
       <c r="A28" s="15" t="s">
         <v>171</v>
       </c>
@@ -3387,36 +3400,36 @@
       <c r="AC28" s="15"/>
       <c r="AD28" s="15"/>
     </row>
-    <row r="38" ht="24.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="50" ht="24.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="60" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="71" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="73" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="76" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="83" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="84" ht="24.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="86" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="88" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="93" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="99" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="102" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="103" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="104" ht="24.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="114" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="115" ht="24.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="117" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="118" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="119" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="120" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" ht="24.75" customHeight="1"/>
+    <row r="39" ht="25.5" customHeight="1"/>
+    <row r="40" ht="25.5" customHeight="1"/>
+    <row r="41" ht="25.5" customHeight="1"/>
+    <row r="42" ht="25.5" customHeight="1"/>
+    <row r="43" ht="25.5" customHeight="1"/>
+    <row r="44" ht="25.5" customHeight="1"/>
+    <row r="50" ht="24.75" customHeight="1"/>
+    <row r="67" ht="60" customHeight="1"/>
+    <row r="71" ht="15" customHeight="1"/>
+    <row r="72" ht="25.5" customHeight="1"/>
+    <row r="73" ht="25.5" customHeight="1"/>
+    <row r="75" ht="25.5" customHeight="1"/>
+    <row r="76" ht="25.5" customHeight="1"/>
+    <row r="78" ht="25.5" customHeight="1"/>
+    <row r="83" ht="15" customHeight="1"/>
+    <row r="84" ht="24.75" customHeight="1"/>
+    <row r="86" ht="15" customHeight="1"/>
+    <row r="88" ht="15" customHeight="1"/>
+    <row r="93" ht="15" customHeight="1"/>
+    <row r="99" ht="15" customHeight="1"/>
+    <row r="102" ht="15" customHeight="1"/>
+    <row r="103" ht="15" customHeight="1"/>
+    <row r="104" ht="24.75" customHeight="1"/>
+    <row r="114" ht="15" customHeight="1"/>
+    <row r="115" ht="24.75" customHeight="1"/>
+    <row r="117" ht="25.5" customHeight="1"/>
+    <row r="118" ht="25.5" customHeight="1"/>
+    <row r="119" ht="25.5" customHeight="1"/>
+    <row r="120" ht="25.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A28:AD28"/>
@@ -3431,18 +3444,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0F0F38-248D-440C-946B-9DDADE2A5CA3}">
   <dimension ref="A2:AU35"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="AG15" sqref="AG15"/>
+    <sheetView tabSelected="1" topLeftCell="AD12" zoomScale="67" workbookViewId="0">
+      <selection activeCell="AO22" sqref="AO22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="23" max="23" width="19.54296875" customWidth="1"/>
     <col min="29" max="29" width="22.453125" customWidth="1"/>
     <col min="32" max="32" width="34.1796875" customWidth="1"/>
+    <col min="41" max="41" width="22.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:47">
       <c r="A2" s="16" t="s">
         <v>172</v>
       </c>
@@ -3493,7 +3507,7 @@
       <c r="AT2" s="16"/>
       <c r="AU2" s="16"/>
     </row>
-    <row r="8" spans="1:47" ht="15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" ht="15">
       <c r="A8" s="14" t="s">
         <v>173</v>
       </c>
@@ -3531,7 +3545,7 @@
       <c r="AK8" s="13"/>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:47" ht="25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" ht="25">
       <c r="A9" s="8" t="s">
         <v>1</v>
       </c>
@@ -3623,7 +3637,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:47" ht="39" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" ht="39">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -3715,7 +3729,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:47" ht="39" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" ht="39">
       <c r="A11" s="4" t="s">
         <v>51</v>
       </c>
@@ -3807,7 +3821,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:47" ht="39" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" ht="39">
       <c r="A12" s="4" t="s">
         <v>70</v>
       </c>
@@ -3899,7 +3913,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:47" ht="39" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" ht="39">
       <c r="A13" s="4" t="s">
         <v>85</v>
       </c>
@@ -3976,7 +3990,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:47" ht="39" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" ht="39">
       <c r="A14" s="4" t="s">
         <v>99</v>
       </c>
@@ -4053,7 +4067,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:47" ht="39" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" ht="39">
       <c r="A15" s="4" t="s">
         <v>112</v>
       </c>
@@ -4130,7 +4144,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47">
       <c r="Y16" s="5" t="s">
         <v>211</v>
       </c>
@@ -4147,7 +4161,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="7:41" x14ac:dyDescent="0.35">
+    <row r="17" spans="7:41">
       <c r="Y17" s="5" t="s">
         <v>218</v>
       </c>
@@ -4164,7 +4178,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="7:41" x14ac:dyDescent="0.35">
+    <row r="18" spans="7:41">
       <c r="Y18" s="5" t="s">
         <v>225</v>
       </c>
@@ -4181,7 +4195,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="20" spans="7:41" ht="15" x14ac:dyDescent="0.35">
+    <row r="20" spans="7:41" ht="15">
       <c r="G20" s="14" t="s">
         <v>193</v>
       </c>
@@ -4196,7 +4210,7 @@
       <c r="AN20" s="13"/>
       <c r="AO20" s="13"/>
     </row>
-    <row r="21" spans="7:41" ht="25" x14ac:dyDescent="0.35">
+    <row r="21" spans="7:41" ht="25">
       <c r="G21" s="8" t="s">
         <v>125</v>
       </c>
@@ -4225,7 +4239,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="7:41" ht="15" x14ac:dyDescent="0.35">
+    <row r="22" spans="7:41" ht="15">
       <c r="G22" s="4" t="s">
         <v>28</v>
       </c>
@@ -4257,11 +4271,11 @@
       <c r="AN22" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="AO22" s="5" t="s">
+      <c r="AO22" s="21" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="7:41" ht="15" x14ac:dyDescent="0.35">
+    <row r="23" spans="7:41" ht="15">
       <c r="G23" s="4" t="s">
         <v>28</v>
       </c>
@@ -4306,11 +4320,11 @@
       <c r="AN23" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="AO23" s="5" t="s">
+      <c r="AO23" s="22" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="7:41" x14ac:dyDescent="0.35">
+    <row r="24" spans="7:41">
       <c r="G24" s="4" t="s">
         <v>28</v>
       </c>
@@ -4359,11 +4373,11 @@
       <c r="AN24" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="AO24" s="5" t="s">
+      <c r="AO24" s="22" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="7:41" x14ac:dyDescent="0.35">
+    <row r="25" spans="7:41">
       <c r="G25" s="4" t="s">
         <v>51</v>
       </c>
@@ -4416,7 +4430,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="26" spans="7:41" x14ac:dyDescent="0.35">
+    <row r="26" spans="7:41">
       <c r="G26" s="4" t="s">
         <v>70</v>
       </c>
@@ -4469,7 +4483,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="27" spans="7:41" x14ac:dyDescent="0.35">
+    <row r="27" spans="7:41">
       <c r="G27" s="4" t="s">
         <v>70</v>
       </c>
@@ -4522,7 +4536,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="7:41" x14ac:dyDescent="0.35">
+    <row r="28" spans="7:41">
       <c r="G28" s="4" t="s">
         <v>85</v>
       </c>
@@ -4575,7 +4589,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="7:41" x14ac:dyDescent="0.35">
+    <row r="29" spans="7:41">
       <c r="G29" s="4" t="s">
         <v>99</v>
       </c>
@@ -4619,7 +4633,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="7:41" x14ac:dyDescent="0.35">
+    <row r="30" spans="7:41">
       <c r="G30" s="4" t="s">
         <v>112</v>
       </c>
@@ -4648,7 +4662,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="7:32" x14ac:dyDescent="0.35">
+    <row r="35" spans="7:32">
       <c r="G35" s="17"/>
       <c r="H35" s="17"/>
       <c r="I35" s="17"/>
@@ -4696,23 +4710,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BCA733-7DF5-4AFE-8941-3220221FE959}">
   <dimension ref="A2:AU57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F23" zoomScale="72" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView topLeftCell="M43" zoomScale="72" workbookViewId="0">
+      <selection activeCell="X48" sqref="X48:X50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="5" max="5" width="34.1796875" customWidth="1"/>
     <col min="11" max="11" width="21.08984375" customWidth="1"/>
+    <col min="13" max="13" width="13.54296875" customWidth="1"/>
     <col min="15" max="15" width="24.453125" customWidth="1"/>
     <col min="17" max="17" width="16" customWidth="1"/>
     <col min="19" max="19" width="15.1796875" customWidth="1"/>
+    <col min="23" max="23" width="19.36328125" customWidth="1"/>
     <col min="24" max="24" width="19.54296875" customWidth="1"/>
+    <col min="29" max="29" width="20.08984375" customWidth="1"/>
+    <col min="30" max="30" width="16.36328125" customWidth="1"/>
+    <col min="31" max="31" width="21.36328125" customWidth="1"/>
+    <col min="32" max="32" width="15.81640625" customWidth="1"/>
     <col min="33" max="33" width="34.54296875" customWidth="1"/>
     <col min="34" max="34" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:47" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:47" ht="15.5">
       <c r="A2" s="18" t="s">
         <v>248</v>
       </c>
@@ -4763,7 +4783,7 @@
       <c r="AT2" s="18"/>
       <c r="AU2" s="18"/>
     </row>
-    <row r="7" spans="1:47" ht="15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" ht="15">
       <c r="L7" s="19" t="s">
         <v>249</v>
       </c>
@@ -4775,7 +4795,7 @@
       <c r="S7" s="19"/>
       <c r="T7" s="19"/>
     </row>
-    <row r="8" spans="1:47" ht="25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" ht="25">
       <c r="C8" s="19" t="s">
         <v>251</v>
       </c>
@@ -4810,7 +4830,7 @@
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
     </row>
-    <row r="9" spans="1:47" ht="26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" ht="26">
       <c r="C9" s="7" t="s">
         <v>259</v>
       </c>
@@ -4868,7 +4888,7 @@
       <c r="AF9" s="13"/>
       <c r="AG9" s="13"/>
     </row>
-    <row r="10" spans="1:47" ht="26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" ht="26">
       <c r="C10" s="2" t="s">
         <v>268</v>
       </c>
@@ -4930,7 +4950,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:47" ht="26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" ht="26">
       <c r="C11" s="2" t="s">
         <v>275</v>
       </c>
@@ -4992,7 +5012,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:47" ht="26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" ht="26">
       <c r="C12" s="2" t="s">
         <v>282</v>
       </c>
@@ -5054,7 +5074,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:47" ht="26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" ht="26">
       <c r="L13" s="2" t="s">
         <v>288</v>
       </c>
@@ -5101,18 +5121,9 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:47" ht="26" x14ac:dyDescent="0.35">
-      <c r="L14" s="2" t="s">
+    <row r="14" spans="1:47">
+      <c r="R14" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>293</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>120</v>
@@ -5121,7 +5132,7 @@
         <v>288</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="X14" s="2" t="s">
         <v>104</v>
@@ -5133,7 +5144,7 @@
         <v>273</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AB14" s="2" t="s">
         <v>290</v>
@@ -5148,9 +5159,9 @@
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:47" ht="26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" ht="26">
       <c r="W15" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="X15" s="2" t="s">
         <v>117</v>
@@ -5165,12 +5176,12 @@
         <v>281</v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="19" spans="6:33" ht="15" x14ac:dyDescent="0.35">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="6:33" ht="15">
       <c r="F19" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
@@ -5178,7 +5189,7 @@
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
     </row>
-    <row r="20" spans="6:33" ht="25" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:33" ht="25">
       <c r="F20" s="7" t="s">
         <v>1</v>
       </c>
@@ -5189,16 +5200,16 @@
         <v>3</v>
       </c>
       <c r="I20" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>298</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>299</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="21" spans="6:33" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:33">
       <c r="F21" s="1" t="s">
         <v>28</v>
       </c>
@@ -5218,7 +5229,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="22" spans="6:33" ht="15" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:33" ht="15">
       <c r="F22" s="1" t="s">
         <v>51</v>
       </c>
@@ -5238,19 +5249,19 @@
         <v>279</v>
       </c>
       <c r="N22" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O22" s="19"/>
       <c r="R22" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S22" s="19"/>
       <c r="V22" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="W22" s="13"/>
       <c r="AB22" s="20" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AC22" s="20"/>
       <c r="AD22" s="20"/>
@@ -5258,7 +5269,7 @@
       <c r="AF22" s="20"/>
       <c r="AG22" s="20"/>
     </row>
-    <row r="23" spans="6:33" ht="25" x14ac:dyDescent="0.35">
+    <row r="23" spans="6:33" ht="25">
       <c r="F23" s="1" t="s">
         <v>70</v>
       </c>
@@ -5290,31 +5301,31 @@
         <v>203</v>
       </c>
       <c r="V23" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="W23" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AB23" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AC23" s="7" t="s">
         <v>125</v>
       </c>
       <c r="AD23" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AE23" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="AF23" s="7" t="s">
         <v>203</v>
       </c>
       <c r="AG23" s="10" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="24" spans="6:33" ht="26" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="24" spans="6:33" ht="26">
       <c r="F24" s="1" t="s">
         <v>85</v>
       </c>
@@ -5340,7 +5351,7 @@
         <v>38</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="S24" s="2" t="s">
         <v>49</v>
@@ -5352,7 +5363,7 @@
         <v>206</v>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="AC24" s="2" t="s">
         <v>28</v>
@@ -5364,13 +5375,13 @@
         <v>43</v>
       </c>
       <c r="AF24" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AG24" s="6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="25" spans="6:33" ht="26" x14ac:dyDescent="0.35">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="25" spans="6:33" ht="26">
       <c r="F25" s="1" t="s">
         <v>99</v>
       </c>
@@ -5387,7 +5398,7 @@
         <v>187</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>280</v>
@@ -5408,25 +5419,25 @@
         <v>214</v>
       </c>
       <c r="AB25" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AC25" s="2" t="s">
         <v>70</v>
       </c>
       <c r="AD25" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AE25" s="2" t="s">
         <v>79</v>
       </c>
       <c r="AF25" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AG25" s="6" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="26" spans="6:33" ht="26" x14ac:dyDescent="0.35">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="26" spans="6:33" ht="26">
       <c r="F26" s="1" t="s">
         <v>112</v>
       </c>
@@ -5443,7 +5454,7 @@
         <v>185</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>287</v>
@@ -5464,25 +5475,25 @@
         <v>220</v>
       </c>
       <c r="AB26" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AC26" s="2" t="s">
         <v>28</v>
       </c>
       <c r="AD26" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="AE26" s="2" t="s">
         <v>43</v>
       </c>
       <c r="AF26" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AG26" s="6" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="27" spans="6:33" ht="39" x14ac:dyDescent="0.35">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="27" spans="6:33" ht="39">
       <c r="V27" s="4" t="s">
         <v>190</v>
       </c>
@@ -5490,25 +5501,25 @@
         <v>227</v>
       </c>
       <c r="AB27" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AC27" s="2" t="s">
         <v>99</v>
       </c>
       <c r="AD27" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AE27" s="2" t="s">
         <v>108</v>
       </c>
       <c r="AF27" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AG27" s="6" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="28" spans="6:33" x14ac:dyDescent="0.35">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="28" spans="6:33">
       <c r="V28" s="4" t="s">
         <v>191</v>
       </c>
@@ -5516,9 +5527,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="6:33" ht="15" x14ac:dyDescent="0.35">
+    <row r="29" spans="6:33" ht="15">
       <c r="P29" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Q29" s="20"/>
       <c r="V29" s="4" t="s">
@@ -5528,48 +5539,48 @@
         <v>236</v>
       </c>
     </row>
-    <row r="30" spans="6:33" ht="25" x14ac:dyDescent="0.35">
+    <row r="30" spans="6:33" ht="25">
       <c r="P30" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Q30" s="7" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="6:33" x14ac:dyDescent="0.35">
+    <row r="31" spans="6:33">
       <c r="P31" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q31" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="6:33" x14ac:dyDescent="0.35">
+    <row r="32" spans="6:33">
       <c r="P32" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q32" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="6:34" x14ac:dyDescent="0.35">
+    <row r="33" spans="6:34">
       <c r="P33" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q33" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="6:34" ht="15" x14ac:dyDescent="0.35">
+    <row r="35" spans="6:34" ht="15">
       <c r="F35" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
       <c r="AB35" s="20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AC35" s="20"/>
       <c r="AD35" s="20"/>
@@ -5578,7 +5589,7 @@
       <c r="AG35" s="20"/>
       <c r="AH35" s="20"/>
     </row>
-    <row r="36" spans="6:34" ht="25" x14ac:dyDescent="0.35">
+    <row r="36" spans="6:34" ht="25">
       <c r="F36" s="7" t="s">
         <v>126</v>
       </c>
@@ -5592,13 +5603,13 @@
         <v>198</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AB36" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AC36" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AD36" s="7" t="s">
         <v>25</v>
@@ -5607,16 +5618,16 @@
         <v>26</v>
       </c>
       <c r="AF36" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AG36" s="7" t="s">
-        <v>321</v>
+        <v>369</v>
       </c>
       <c r="AH36" s="10" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="37" spans="6:34" ht="15" x14ac:dyDescent="0.35">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="37" spans="6:34" ht="15">
       <c r="F37" s="1" t="s">
         <v>135</v>
       </c>
@@ -5630,7 +5641,7 @@
         <v>43</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="T37" s="13" t="s">
         <v>175</v>
@@ -5638,7 +5649,7 @@
       <c r="U37" s="13"/>
       <c r="V37" s="13"/>
       <c r="AB37" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AC37" s="2" t="s">
         <v>272</v>
@@ -5652,14 +5663,14 @@
       <c r="AF37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AG37" s="2" t="s">
-        <v>213</v>
+      <c r="AG37" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="AH37" s="6" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="38" spans="6:34" ht="25" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="38" spans="6:34">
       <c r="F38" s="1" t="s">
         <v>141</v>
       </c>
@@ -5673,19 +5684,19 @@
         <v>43</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="T38" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="U38" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="V38" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AB38" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AC38" s="2" t="s">
         <v>279</v>
@@ -5699,14 +5710,14 @@
       <c r="AF38" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AG38" s="2" t="s">
-        <v>219</v>
+      <c r="AG38" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="AH38" s="6" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="39" spans="6:34" ht="15" x14ac:dyDescent="0.35">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="39" spans="6:34" ht="15">
       <c r="F39" s="1" t="s">
         <v>142</v>
       </c>
@@ -5720,10 +5731,10 @@
         <v>43</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M39" s="19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N39" s="19"/>
       <c r="O39" s="19"/>
@@ -5739,7 +5750,7 @@
         <v>36</v>
       </c>
       <c r="AB39" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="AC39" s="2" t="s">
         <v>286</v>
@@ -5753,14 +5764,14 @@
       <c r="AF39" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AG39" s="2" t="s">
-        <v>213</v>
+      <c r="AG39" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="AH39" s="6" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="40" spans="6:34" ht="25" x14ac:dyDescent="0.35">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="40" spans="6:34" ht="25">
       <c r="F40" s="1" t="s">
         <v>145</v>
       </c>
@@ -5774,10 +5785,10 @@
         <v>66</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="N40" s="7" t="s">
         <v>125</v>
@@ -5801,7 +5812,7 @@
         <v>59</v>
       </c>
       <c r="AB40" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AC40" s="2" t="s">
         <v>291</v>
@@ -5816,13 +5827,13 @@
         <v>86</v>
       </c>
       <c r="AG40" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AH40" s="6" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="41" spans="6:34" ht="26" x14ac:dyDescent="0.35">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="41" spans="6:34">
       <c r="F41" s="1" t="s">
         <v>151</v>
       </c>
@@ -5836,10 +5847,10 @@
         <v>79</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>51</v>
@@ -5863,10 +5874,10 @@
         <v>59</v>
       </c>
       <c r="AB41" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="AC41" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AD41" s="2" t="s">
         <v>39</v>
@@ -5875,16 +5886,16 @@
         <v>49</v>
       </c>
       <c r="AF41" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="AG41" s="2" t="s">
-        <v>219</v>
+        <v>359</v>
+      </c>
+      <c r="AG41" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="AH41" s="6" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="42" spans="6:34" ht="26" x14ac:dyDescent="0.35">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="42" spans="6:34">
       <c r="F42" s="1" t="s">
         <v>155</v>
       </c>
@@ -5898,10 +5909,10 @@
         <v>79</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>85</v>
@@ -5916,10 +5927,10 @@
         <v>97</v>
       </c>
       <c r="AB42" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AC42" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AD42" s="2" t="s">
         <v>49</v>
@@ -5930,14 +5941,14 @@
       <c r="AF42" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AG42" s="2" t="s">
-        <v>213</v>
+      <c r="AG42" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="AH42" s="6" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="43" spans="6:34" x14ac:dyDescent="0.35">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="43" spans="6:34">
       <c r="F43" s="1" t="s">
         <v>157</v>
       </c>
@@ -5951,10 +5962,10 @@
         <v>96</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>112</v>
@@ -5969,7 +5980,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="6:34" x14ac:dyDescent="0.35">
+    <row r="44" spans="6:34">
       <c r="F44" s="1" t="s">
         <v>163</v>
       </c>
@@ -5983,10 +5994,10 @@
         <v>108</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="45" spans="6:34" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="45" spans="6:34">
       <c r="F45" s="1" t="s">
         <v>167</v>
       </c>
@@ -6000,10 +6011,10 @@
         <v>121</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="46" spans="6:34" ht="15" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="46" spans="6:34" ht="15">
       <c r="U46" s="13" t="s">
         <v>196</v>
       </c>
@@ -6018,7 +6029,7 @@
       <c r="AF46" s="13"/>
       <c r="AG46" s="13"/>
     </row>
-    <row r="47" spans="6:34" x14ac:dyDescent="0.35">
+    <row r="47" spans="6:34">
       <c r="U47" s="9" t="s">
         <v>204</v>
       </c>
@@ -6047,7 +6058,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="6:34" x14ac:dyDescent="0.35">
+    <row r="48" spans="6:34">
       <c r="U48" s="5" t="s">
         <v>210</v>
       </c>
@@ -6057,7 +6068,7 @@
       <c r="W48" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="X48" s="5" t="s">
+      <c r="X48" s="21" t="s">
         <v>213</v>
       </c>
       <c r="AC48" s="5" t="s">
@@ -6076,7 +6087,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="10:33" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:33">
       <c r="U49" s="5" t="s">
         <v>217</v>
       </c>
@@ -6086,7 +6097,7 @@
       <c r="W49" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="X49" s="5" t="s">
+      <c r="X49" s="22" t="s">
         <v>219</v>
       </c>
       <c r="AC49" s="5" t="s">
@@ -6105,9 +6116,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="10:33" ht="15" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:33" ht="15">
       <c r="J50" s="20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K50" s="20"/>
       <c r="L50" s="20"/>
@@ -6123,7 +6134,7 @@
       <c r="W50" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="X50" s="5" t="s">
+      <c r="X50" s="22" t="s">
         <v>226</v>
       </c>
       <c r="AC50" s="5" t="s">
@@ -6142,24 +6153,24 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="10:33" ht="25" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:33" ht="25">
       <c r="J51" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K51" s="7" t="s">
         <v>125</v>
       </c>
       <c r="L51" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="M51" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="M51" s="7" t="s">
+      <c r="N51" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="O51" s="10" t="s">
         <v>320</v>
-      </c>
-      <c r="N51" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="O51" s="10" t="s">
-        <v>322</v>
       </c>
       <c r="U51" s="5" t="s">
         <v>231</v>
@@ -6189,24 +6200,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="10:33" ht="26" x14ac:dyDescent="0.35">
+    <row r="52" spans="10:33" ht="26">
       <c r="J52" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="M52" s="1" t="s">
         <v>29</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="O52" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="U52" s="5" t="s">
         <v>234</v>
@@ -6236,24 +6247,24 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="10:33" ht="26" x14ac:dyDescent="0.35">
+    <row r="53" spans="10:33" ht="26">
       <c r="J53" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>51</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="M53" s="1" t="s">
         <v>52</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O53" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="U53" s="5" t="s">
         <v>237</v>
@@ -6283,24 +6294,24 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="10:33" ht="26" x14ac:dyDescent="0.35">
+    <row r="54" spans="10:33" ht="26">
       <c r="J54" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>70</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="M54" s="1" t="s">
         <v>71</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="O54" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="U54" s="5" t="s">
         <v>240</v>
@@ -6330,24 +6341,24 @@
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="10:33" ht="26" x14ac:dyDescent="0.35">
+    <row r="55" spans="10:33" ht="26">
       <c r="J55" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>85</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="M55" s="1" t="s">
         <v>86</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="U55" s="5" t="s">
         <v>243</v>
@@ -6377,24 +6388,24 @@
         <v>242</v>
       </c>
     </row>
-    <row r="56" spans="10:33" ht="26" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:33" ht="26">
       <c r="J56" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>99</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="M56" s="1" t="s">
         <v>100</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O56" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="U56" s="5" t="s">
         <v>246</v>
@@ -6424,24 +6435,24 @@
         <v>245</v>
       </c>
     </row>
-    <row r="57" spans="10:33" ht="26" x14ac:dyDescent="0.35">
+    <row r="57" spans="10:33" ht="26">
       <c r="J57" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>112</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="M57" s="1" t="s">
         <v>113</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="O57" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -6467,5 +6478,6 @@
     <mergeCell ref="F19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>